<commit_message>
Add more markers and add icons to landing page
</commit_message>
<xml_diff>
--- a/volt/docs/power_consumption_data.xlsx
+++ b/volt/docs/power_consumption_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATSivkov21\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Documents\New folder\2324-10-volt-ai-solarcode\volt\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9C386AA-E810-47BE-B7F4-3B6443A67251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F15A04-C3D8-4A2A-9EB1-D1D0E464FC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{BD2ADB95-BECE-4B10-9084-73BE0CFDE515}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{BD2ADB95-BECE-4B10-9084-73BE0CFDE515}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,9 +391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -431,7 +431,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -537,7 +537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -679,7 +679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,17 +689,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D908C2F1-560C-4056-BA51-2F4B01FC7522}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -727,7 +727,7 @@
         <v>553.20000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -741,7 +741,7 @@
         <v>450.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -755,7 +755,7 @@
         <v>343.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -769,7 +769,7 @@
         <v>320.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -783,7 +783,7 @@
         <v>293.10000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -797,7 +797,7 @@
         <v>242.9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -811,7 +811,7 @@
         <v>235.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -825,7 +825,7 @@
         <v>224.1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -839,7 +839,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -853,7 +853,7 @@
         <v>204.2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -867,7 +867,7 @@
         <v>195.6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -881,7 +881,7 @@
         <v>184.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -895,7 +895,7 @@
         <v>176.2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -909,7 +909,7 @@
         <v>168.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -923,7 +923,7 @@
         <v>165.9</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -937,7 +937,7 @@
         <v>159.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -951,7 +951,7 @@
         <v>155.19999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -965,7 +965,7 @@
         <v>149.80000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -979,7 +979,7 @@
         <v>144.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -993,7 +993,7 @@
         <v>139.6</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>

</xml_diff>